<commit_message>
template now works for LOLER Documents
</commit_message>
<xml_diff>
--- a/static/LOLER-ReportTemplate.xlsx
+++ b/static/LOLER-ReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Aaron Gomm\Reports\Lee Lifting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarongomm\Documents\GitHub\project2510\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AE9EBE-4A05-4E53-8935-F7BD06F2E129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9072A94-82E2-43B0-9865-0819A1D404D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lee Lifting - LM67 JXC" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>Serial Number</t>
-  </si>
-  <si>
-    <t>Report ID</t>
-  </si>
-  <si>
-    <t>Equipment Type</t>
-  </si>
-  <si>
-    <t>SWL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Industrial Safety Inspections Ltd</t>
   </si>
@@ -46,70 +34,16 @@
     <t>Job Information</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job Type: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tel: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Contact: </t>
   </si>
   <si>
-    <t xml:space="preserve">Logged: </t>
+    <t>{Client Name}</t>
   </si>
   <si>
-    <t xml:space="preserve">Job Number: </t>
+    <t>{Client Address}</t>
   </si>
   <si>
-    <t>Lee Lifting Services</t>
-  </si>
-  <si>
-    <t>Unit 5 Falcon Way</t>
-  </si>
-  <si>
-    <t>North Feltham Trading Estate</t>
-  </si>
-  <si>
-    <t>Feltham</t>
-  </si>
-  <si>
-    <t>Middlesex</t>
-  </si>
-  <si>
-    <t>TW14 0XJ</t>
-  </si>
-  <si>
-    <t>ISI Number</t>
-  </si>
-  <si>
-    <t>DOM</t>
-  </si>
-  <si>
-    <t>Client Ref</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>A Defect</t>
-  </si>
-  <si>
-    <t>B Defect</t>
-  </si>
-  <si>
-    <t>C Defect</t>
-  </si>
-  <si>
-    <t>D Defect</t>
-  </si>
-  <si>
-    <t>Report Date</t>
-  </si>
-  <si>
-    <t>Next Inspection Date</t>
+    <t>Job Number: {Job Number}</t>
   </si>
 </sst>
 </file>
@@ -668,14 +602,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -689,7 +617,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -735,62 +662,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color rgb="FFFFFF00"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -850,29 +722,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A14:N19" totalsRowShown="0" dataDxfId="15" headerRowBorderDxfId="14">
-  <autoFilter ref="A14:N19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Equipment Type" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ISI Number" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Serial Number" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DOM" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SWL" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Client Ref" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Location" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{ABEBD5A0-93A6-415D-9323-FE4E210B40C4}" name="Report ID" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="A Defect" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="B Defect" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{5611BAE0-8A62-473A-9DFA-2EAE4FA050FF}" name="C Defect" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{3CCEF4D9-BA1E-471E-8070-866826F1D40B}" name="D Defect" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{2490E7F5-86BF-4A4E-83B6-1C0692FCB708}" name="Report Date" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{91FAD56F-C197-4C93-8A49-D061B69F7F6A}" name="Next Inspection Date" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1172,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:N19"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:N14"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,211 +1041,68 @@
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
     </row>
-    <row r="5" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Template update for LOLER, feilds included for additional details have been added.
</commit_message>
<xml_diff>
--- a/static/LOLER-ReportTemplate.xlsx
+++ b/static/LOLER-ReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarongomm\Documents\GitHub\project2510\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9072A94-82E2-43B0-9865-0819A1D404D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC81256-A985-4F90-BB04-DF5F68C38A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Industrial Safety Inspections Ltd</t>
   </si>
@@ -37,13 +37,31 @@
     <t xml:space="preserve">Contact: </t>
   </si>
   <si>
-    <t>{Client Name}</t>
-  </si>
-  <si>
-    <t>{Client Address}</t>
-  </si>
-  <si>
-    <t>Job Number: {Job Number}</t>
+    <t>{{Client_Address_1}}</t>
+  </si>
+  <si>
+    <t>{{Client_Name}}</t>
+  </si>
+  <si>
+    <t>{{Client_Address_2}}</t>
+  </si>
+  <si>
+    <t>{{Client_Postcode}}</t>
+  </si>
+  <si>
+    <t>{{Job_Number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Number: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact No: </t>
+  </si>
+  <si>
+    <t>{{Client_Contact_No}}</t>
+  </si>
+  <si>
+    <t>{{Client_Contact}}</t>
   </si>
 </sst>
 </file>
@@ -602,7 +620,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -617,6 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1024,7 +1043,7 @@
   <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,18 +1079,20 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="B9" s="6"/>
       <c r="C9" s="3" t="s">
         <v>3</v>
@@ -1079,26 +1100,36 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B10" s="6"/>
       <c r="C10" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>